<commit_message>
more structure for website
</commit_message>
<xml_diff>
--- a/material/ENVS363_563_Redesign.xlsx
+++ b/material/ENVS363_563_Redesign.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PIETROST/Library/CloudStorage/Dropbox/GitHub/gds/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PIETROST/Library/CloudStorage/Dropbox/GitHub/gds/material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591BFD0A-C565-FE40-8CED-28A38E1B517B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01845D1C-55CF-A94C-83E5-74BC957914C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="500" windowWidth="29480" windowHeight="21100" xr2:uid="{A2A5BC75-8F53-BE49-8375-DBD12ADBE695}"/>
+    <workbookView xWindow="30480" yWindow="500" windowWidth="29480" windowHeight="21100" xr2:uid="{A2A5BC75-8F53-BE49-8375-DBD12ADBE695}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions_TODOs" sheetId="3" r:id="rId1"/>
     <sheet name="Overview" sheetId="4" r:id="rId2"/>
     <sheet name="Learning_Outcomes" sheetId="1" r:id="rId3"/>
     <sheet name="Assessments" sheetId="2" r:id="rId4"/>
+    <sheet name="random" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>LO1</t>
   </si>
@@ -276,6 +277,36 @@
   <si>
     <t>(point to point, service area analysis, route optimization, select optimal site, ODMs)</t>
   </si>
+  <si>
+    <t>https://github.com/hadley/r4ds/blob/main/_quarto.yml</t>
+  </si>
+  <si>
+    <t>get a better website name</t>
+  </si>
+  <si>
+    <t>Other To Dos</t>
+  </si>
+  <si>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>Demonstratos</t>
+  </si>
+  <si>
+    <t>Matthew Howard</t>
+  </si>
+  <si>
+    <t>Ruth Neville</t>
+  </si>
+  <si>
+    <t>Akos Balog</t>
+  </si>
+  <si>
+    <t>Rodgers Iradukunda</t>
+  </si>
+  <si>
+    <t>https://darribas.org/gds_course/content/home.html</t>
+  </si>
 </sst>
 </file>
 
@@ -400,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -408,11 +439,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -743,265 +773,284 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="15" customWidth="1"/>
-    <col min="7" max="9" width="19.6640625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="32.5" style="15" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="27.5" style="14" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="14" customWidth="1"/>
+    <col min="7" max="9" width="19.6640625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="32.5" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="11" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:10" s="10" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A16" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1072,7 +1121,7 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1083,7 +1132,7 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1094,7 +1143,7 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1105,7 +1154,7 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1116,7 +1165,7 @@
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1124,10 +1173,10 @@
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1170,4 +1219,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFC601F-B707-6D4F-9D3E-E44AD25A22DF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>